<commit_message>
upload upah tidak tetap dikunci hanya bulanan saja. kode 2
</commit_message>
<xml_diff>
--- a/assets/xlsx/tempate_import_upahtt.xlsx
+++ b/assets/xlsx/tempate_import_upahtt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="6760" windowWidth="28060" windowHeight="10160"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -66,18 +66,12 @@
     <t>4. Kolom Masuk Pajak diisi YA atau TIDAK</t>
   </si>
   <si>
-    <t>5. Kode Jenis Upah = 1. Tahunan 2. Bulanan</t>
-  </si>
-  <si>
     <t>6. Kode Fungsi Pajak = 1. Penambah 2. Pengurang 3. Netral</t>
   </si>
   <si>
     <t>Kode Jenis Upah</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>3. Format tangal dd.mm.yyyy. Contoh 01.05.2015</t>
   </si>
   <si>
@@ -91,6 +85,12 @@
   </si>
   <si>
     <t>ABC</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>5. Kode Jenis Upah = 2. Bulanan</t>
   </si>
 </sst>
 </file>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,10 +554,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>6</v>
@@ -580,19 +580,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>9</v>
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -643,7 +643,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -653,12 +653,12 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>